<commit_message>
project 5 final commit
</commit_message>
<xml_diff>
--- a/Project 5/Extension #1 Data Table.xlsx
+++ b/Project 5/Extension #1 Data Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/Northeastern Khoury/CS5330 Pattern Recognition &amp; Computer Vision/Projects/Project 5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E29C4A-E86C-6F45-A26F-1142D1C90B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CBB810-CDF6-F740-8CFF-15DC065C3F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{A96BC008-9A93-CD4F-B7BD-27D10476617C}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>